<commit_message>
Added technologies comparison Excel
</commit_message>
<xml_diff>
--- a/Allegati/Comparazione tecnologie.xlsx
+++ b/Allegati/Comparazione tecnologie.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20382"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paolo.forgia\workspace\CPTRoverControl\Allegati\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paolo\workspace\CPTRoverControl\Allegati\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C049E717-1988-412A-B19C-3AFD0127BAC3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC00F20D-BCF2-4E9C-AF1A-8AC4A2ECB10F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{9C3C02D9-B871-4DD8-B30D-27A873B679FB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9C3C02D9-B871-4DD8-B30D-27A873B679FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -42,29 +42,29 @@
     <t>Gestione orientamento dispositivo</t>
   </si>
   <si>
-    <t>Molto complessa</t>
-  </si>
-  <si>
     <t>Semplice</t>
   </si>
   <si>
-    <t>Bassa</t>
-  </si>
-  <si>
-    <t>Alta (emulazione richiede circa 16GB di RAM)</t>
-  </si>
-  <si>
     <t>Invio/Ricezione dati via Bluetooth</t>
   </si>
   <si>
-    <t>Medio-semplice</t>
+    <t>Basso</t>
+  </si>
+  <si>
+    <t>Alto (emulazione richiede circa 16GB di RAM)</t>
+  </si>
+  <si>
+    <t>Molto complesso</t>
+  </si>
+  <si>
+    <t>Medio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,54 +73,79 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <strike/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -132,23 +157,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="3" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Bad" xfId="4" builtinId="27"/>
+    <cellStyle name="Good" xfId="3" builtinId="26"/>
+    <cellStyle name="Heading 4" xfId="2" builtinId="19"/>
+    <cellStyle name="Neutral" xfId="5" builtinId="28"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Title" xfId="1" builtinId="15"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -164,7 +200,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -460,7 +496,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56E101AC-BCEE-43C8-B5F3-321C6F79CD2C}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -468,75 +504,72 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" style="1" customWidth="1"/>
-    <col min="2" max="3" width="43.85546875" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" style="8" customWidth="1"/>
+    <col min="2" max="3" width="47.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:4" s="7" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="8"/>
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="6" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="7"/>
+      <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="2"/>
-    </row>
-    <row r="9" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
+      <c r="B7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>